<commit_message>
Committed Changes on 2022-01-04
</commit_message>
<xml_diff>
--- a/A3_Project_Demo_Digital_Transformation/Results_Data/Step4_Results_Ouput/2_Line_of_Defense/output_ad_xyz_ManagerReview_20211230_Debra.Emp21@xyz.com.xlsx
+++ b/A3_Project_Demo_Digital_Transformation/Results_Data/Step4_Results_Ouput/2_Line_of_Defense/output_ad_xyz_ManagerReview_20211230_Debra.Emp21@xyz.com.xlsx
@@ -17,112 +17,124 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="84">
   <si>
+    <t>AD_Privileged_Access</t>
+  </si>
+  <si>
+    <t>HR_Department_Name</t>
+  </si>
+  <si>
+    <t>HR_Manage_Email</t>
+  </si>
+  <si>
+    <t>AD_Lastname</t>
+  </si>
+  <si>
     <t>HR_Last_Name</t>
   </si>
   <si>
+    <t>zMatched</t>
+  </si>
+  <si>
+    <t>AD_Unique_AD_Departments</t>
+  </si>
+  <si>
+    <t>AD_WhenChanged</t>
+  </si>
+  <si>
+    <t>HR_Record_Type</t>
+  </si>
+  <si>
+    <t>AD_AccountExpiry</t>
+  </si>
+  <si>
+    <t>AD_EmailAddress</t>
+  </si>
+  <si>
+    <t>AD_Firstname</t>
+  </si>
+  <si>
+    <t>AD_Enabled</t>
+  </si>
+  <si>
+    <t>AD_DisplayName</t>
+  </si>
+  <si>
     <t>HR_Work_Email</t>
   </si>
   <si>
+    <t>AD_xyz_Grp_Tags</t>
+  </si>
+  <si>
+    <t>HR_Status</t>
+  </si>
+  <si>
+    <t>AD_Passwordset</t>
+  </si>
+  <si>
+    <t>HR_Termination_Date</t>
+  </si>
+  <si>
+    <t>AD_Description</t>
+  </si>
+  <si>
+    <t>HR_Employee_No</t>
+  </si>
+  <si>
+    <t>zDays_SinceLastLogonDate</t>
+  </si>
+  <si>
     <t>AD_CreateTimeStamp</t>
   </si>
   <si>
+    <t>AD_Company</t>
+  </si>
+  <si>
+    <t>AD_Department</t>
+  </si>
+  <si>
+    <t>AD_WhenCreated</t>
+  </si>
+  <si>
+    <t>zDays_SincePswdReset</t>
+  </si>
+  <si>
+    <t>zDays_SinceWhenCreated</t>
+  </si>
+  <si>
+    <t>zAD_User_Status</t>
+  </si>
+  <si>
+    <t>AD_SamAccountName</t>
+  </si>
+  <si>
+    <t>HR_First_Name</t>
+  </si>
+  <si>
+    <t>zDays_SinceWhenChanged</t>
+  </si>
+  <si>
+    <t>AD_LastLogonDate</t>
+  </si>
+  <si>
+    <t>HR_Division</t>
+  </si>
+  <si>
     <t>zTerminated_User_ActiveAD</t>
   </si>
   <si>
-    <t>zDays_SinceWhenCreated</t>
-  </si>
-  <si>
-    <t>HR_Record_Type</t>
-  </si>
-  <si>
-    <t>AD_Privileged_Access</t>
-  </si>
-  <si>
-    <t>AD_AccountExpiry</t>
-  </si>
-  <si>
-    <t>AD_WhenCreated</t>
-  </si>
-  <si>
-    <t>AD_WhenChanged</t>
-  </si>
-  <si>
-    <t>AD_xyz_Grp_Tags</t>
-  </si>
-  <si>
-    <t>zAD_User_Status</t>
-  </si>
-  <si>
-    <t>AD_Passwordset</t>
-  </si>
-  <si>
-    <t>AD_Company</t>
-  </si>
-  <si>
-    <t>AD_SamAccountName</t>
-  </si>
-  <si>
-    <t>AD_Unique_AD_Departments</t>
-  </si>
-  <si>
-    <t>AD_Department</t>
-  </si>
-  <si>
-    <t>HR_Division</t>
-  </si>
-  <si>
-    <t>HR_First_Name</t>
-  </si>
-  <si>
-    <t>AD_Firstname</t>
-  </si>
-  <si>
-    <t>HR_Department_Name</t>
-  </si>
-  <si>
-    <t>HR_Employee_No</t>
-  </si>
-  <si>
-    <t>HR_Termination_Date</t>
-  </si>
-  <si>
-    <t>zDays_SinceWhenChanged</t>
-  </si>
-  <si>
     <t>AD_xyz_Dept_Tags</t>
   </si>
   <si>
-    <t>zMatched</t>
-  </si>
-  <si>
-    <t>AD_Lastname</t>
-  </si>
-  <si>
-    <t>zDays_SincePswdReset</t>
-  </si>
-  <si>
-    <t>AD_Enabled</t>
-  </si>
-  <si>
-    <t>AD_EmailAddress</t>
-  </si>
-  <si>
-    <t>AD_Description</t>
-  </si>
-  <si>
-    <t>zDays_SinceLastLogonDate</t>
-  </si>
-  <si>
-    <t>AD_LastLogonDate</t>
-  </si>
-  <si>
-    <t>HR_Manage_Email</t>
-  </si>
-  <si>
-    <t>HR_Status</t>
-  </si>
-  <si>
-    <t>AD_DisplayName</t>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>AWS</t>
+  </si>
+  <si>
+    <t>CRM product</t>
+  </si>
+  <si>
+    <t>Debra.Emp21@xyz.com</t>
   </si>
   <si>
     <t>Emp15</t>
@@ -137,6 +149,15 @@
     <t>Emp24</t>
   </si>
   <si>
+    <t>HR_Match</t>
+  </si>
+  <si>
+    <t>XY-Dept2</t>
+  </si>
+  <si>
+    <t>XYZ Employee</t>
+  </si>
+  <si>
     <t>pal.emp15@xyz.com</t>
   </si>
   <si>
@@ -149,10 +170,31 @@
     <t>clare.emp24@xyz.com</t>
   </si>
   <si>
-    <t>XYZ Employee</t>
-  </si>
-  <si>
-    <t>yes</t>
+    <t>Pal</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Stefani</t>
+  </si>
+  <si>
+    <t>Clare</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>Pal Emp15</t>
+  </si>
+  <si>
+    <t>Robert Emp22</t>
+  </si>
+  <si>
+    <t>Stefani Emp23</t>
+  </si>
+  <si>
+    <t>Clare Emp24</t>
   </si>
   <si>
     <t>X</t>
@@ -161,6 +203,21 @@
     <t>Active</t>
   </si>
   <si>
+    <t>Leave</t>
+  </si>
+  <si>
+    <t>Request#109</t>
+  </si>
+  <si>
+    <t>Request#102</t>
+  </si>
+  <si>
+    <t>Request#101</t>
+  </si>
+  <si>
+    <t>Request#100</t>
+  </si>
+  <si>
     <t>PALEMP15x</t>
   </si>
   <si>
@@ -173,9 +230,6 @@
     <t>CLAREEMP24x</t>
   </si>
   <si>
-    <t>XY-Dept2</t>
-  </si>
-  <si>
     <t>Consulting</t>
   </si>
   <si>
@@ -183,60 +237,6 @@
   </si>
   <si>
     <t>Data &amp; Analytics</t>
-  </si>
-  <si>
-    <t>Pal</t>
-  </si>
-  <si>
-    <t>Robert</t>
-  </si>
-  <si>
-    <t>Stefani</t>
-  </si>
-  <si>
-    <t>Clare</t>
-  </si>
-  <si>
-    <t>AWS</t>
-  </si>
-  <si>
-    <t>CRM product</t>
-  </si>
-  <si>
-    <t>HR_Match</t>
-  </si>
-  <si>
-    <t>True</t>
-  </si>
-  <si>
-    <t>Request#109</t>
-  </si>
-  <si>
-    <t>Request#102</t>
-  </si>
-  <si>
-    <t>Request#101</t>
-  </si>
-  <si>
-    <t>Request#100</t>
-  </si>
-  <si>
-    <t>Debra.Emp21@xyz.com</t>
-  </si>
-  <si>
-    <t>Leave</t>
-  </si>
-  <si>
-    <t>Pal Emp15</t>
-  </si>
-  <si>
-    <t>Robert Emp22</t>
-  </si>
-  <si>
-    <t>Stefani Emp23</t>
-  </si>
-  <si>
-    <t>Clare Emp24</t>
   </si>
   <si>
     <t>AD_Group</t>
@@ -748,80 +748,86 @@
       <c r="A2" s="1">
         <v>67</v>
       </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
       <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="2">
+      <c r="F2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" s="2">
+        <v>44459.5591087963</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>60</v>
+      </c>
+      <c r="R2" t="s">
+        <v>61</v>
+      </c>
+      <c r="S2" s="2">
+        <v>44456.52199074074</v>
+      </c>
+      <c r="U2" t="s">
+        <v>63</v>
+      </c>
+      <c r="V2">
+        <v>1015</v>
+      </c>
+      <c r="W2">
+        <v>106</v>
+      </c>
+      <c r="X2" s="2">
         <v>44457.52199074074</v>
       </c>
-      <c r="F2">
+      <c r="Z2" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA2" s="2">
+        <v>44457.52199074074</v>
+      </c>
+      <c r="AB2">
+        <v>109</v>
+      </c>
+      <c r="AC2">
         <v>108</v>
       </c>
-      <c r="G2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44457.52199074074</v>
-      </c>
-      <c r="K2" s="2">
-        <v>44459.5591087963</v>
-      </c>
-      <c r="L2" t="s">
-        <v>46</v>
-      </c>
-      <c r="M2" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="2">
-        <v>44456.52199074074</v>
-      </c>
-      <c r="P2" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" t="s">
-        <v>52</v>
-      </c>
-      <c r="S2" t="s">
-        <v>53</v>
-      </c>
-      <c r="T2" t="s">
-        <v>56</v>
-      </c>
-      <c r="U2" t="s">
-        <v>56</v>
-      </c>
-      <c r="V2" t="s">
-        <v>60</v>
-      </c>
-      <c r="W2">
-        <v>1015</v>
-      </c>
-      <c r="Y2">
-        <v>106</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2">
-        <v>109</v>
-      </c>
       <c r="AD2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="AE2" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="AF2" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="AG2">
         <v>106</v>
@@ -830,13 +836,7 @@
         <v>44459.54693287037</v>
       </c>
       <c r="AI2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:37">
@@ -844,16 +844,19 @@
         <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="2">
-        <v>44457.52199074074</v>
-      </c>
-      <c r="F3">
-        <v>108</v>
+      <c r="F3" t="s">
+        <v>41</v>
       </c>
       <c r="G3" t="s">
         <v>44</v>
@@ -861,65 +864,68 @@
       <c r="H3" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="2">
+      <c r="I3" s="2">
+        <v>44459.5591087963</v>
+      </c>
+      <c r="J3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" t="s">
+        <v>55</v>
+      </c>
+      <c r="O3" t="s">
+        <v>57</v>
+      </c>
+      <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R3" t="s">
+        <v>61</v>
+      </c>
+      <c r="S3" s="2">
+        <v>44456.52199074074</v>
+      </c>
+      <c r="U3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V3">
+        <v>1022</v>
+      </c>
+      <c r="W3">
+        <v>106</v>
+      </c>
+      <c r="X3" s="2">
         <v>44457.52199074074</v>
       </c>
-      <c r="K3" s="2">
-        <v>44459.5591087963</v>
-      </c>
-      <c r="L3" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="2">
-        <v>44456.52199074074</v>
-      </c>
-      <c r="P3" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="Z3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA3" s="2">
+        <v>44457.52199074074</v>
+      </c>
+      <c r="AB3">
+        <v>109</v>
+      </c>
+      <c r="AC3">
+        <v>108</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF3" t="s">
         <v>52</v>
-      </c>
-      <c r="R3" t="s">
-        <v>52</v>
-      </c>
-      <c r="S3" t="s">
-        <v>54</v>
-      </c>
-      <c r="T3" t="s">
-        <v>57</v>
-      </c>
-      <c r="U3" t="s">
-        <v>57</v>
-      </c>
-      <c r="V3" t="s">
-        <v>61</v>
-      </c>
-      <c r="W3">
-        <v>1022</v>
-      </c>
-      <c r="Y3">
-        <v>106</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AC3">
-        <v>109</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>65</v>
       </c>
       <c r="AG3">
         <v>106</v>
@@ -928,13 +934,7 @@
         <v>44459.54693287037</v>
       </c>
       <c r="AI3" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:37">
@@ -942,16 +942,19 @@
         <v>124</v>
       </c>
       <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
         <v>42</v>
       </c>
-      <c r="D4" s="2">
-        <v>44457.52199074074</v>
-      </c>
-      <c r="F4">
-        <v>108</v>
+      <c r="F4" t="s">
+        <v>42</v>
       </c>
       <c r="G4" t="s">
         <v>44</v>
@@ -959,65 +962,68 @@
       <c r="H4" t="s">
         <v>45</v>
       </c>
-      <c r="J4" s="2">
+      <c r="I4" s="2">
+        <v>44459.5591087963</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" t="s">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s">
+        <v>53</v>
+      </c>
+      <c r="N4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" t="s">
+        <v>58</v>
+      </c>
+      <c r="P4" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>60</v>
+      </c>
+      <c r="R4" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="2">
+        <v>44456.52199074074</v>
+      </c>
+      <c r="U4" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4">
+        <v>1023</v>
+      </c>
+      <c r="W4">
+        <v>106</v>
+      </c>
+      <c r="X4" s="2">
         <v>44457.52199074074</v>
       </c>
-      <c r="K4" s="2">
-        <v>44459.5591087963</v>
-      </c>
-      <c r="L4" t="s">
-        <v>46</v>
-      </c>
-      <c r="M4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" s="2">
-        <v>44456.52199074074</v>
-      </c>
-      <c r="P4" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>52</v>
-      </c>
-      <c r="R4" t="s">
-        <v>52</v>
-      </c>
-      <c r="S4" t="s">
-        <v>54</v>
-      </c>
-      <c r="T4" t="s">
-        <v>58</v>
-      </c>
-      <c r="U4" t="s">
-        <v>58</v>
-      </c>
-      <c r="V4" t="s">
+      <c r="Z4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA4" s="2">
+        <v>44457.52199074074</v>
+      </c>
+      <c r="AB4">
+        <v>109</v>
+      </c>
+      <c r="AC4">
+        <v>108</v>
+      </c>
+      <c r="AD4" t="s">
         <v>61</v>
       </c>
-      <c r="W4">
-        <v>1023</v>
-      </c>
-      <c r="Y4">
-        <v>106</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC4">
-        <v>109</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>63</v>
-      </c>
       <c r="AE4" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="AF4" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="AG4">
         <v>106</v>
@@ -1026,12 +1032,6 @@
         <v>44459.54693287037</v>
       </c>
       <c r="AI4" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK4" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1040,76 +1040,82 @@
         <v>133</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="2">
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="2">
+        <v>44459.5591087963</v>
+      </c>
+      <c r="J5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M5" t="s">
+        <v>54</v>
+      </c>
+      <c r="N5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O5" t="s">
+        <v>59</v>
+      </c>
+      <c r="P5" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>60</v>
+      </c>
+      <c r="R5" t="s">
+        <v>61</v>
+      </c>
+      <c r="S5" s="2">
+        <v>44456.52199074074</v>
+      </c>
+      <c r="U5" t="s">
+        <v>66</v>
+      </c>
+      <c r="V5">
+        <v>1024</v>
+      </c>
+      <c r="W5">
+        <v>106</v>
+      </c>
+      <c r="X5" s="2">
         <v>44457.52199074074</v>
       </c>
-      <c r="F5">
+      <c r="AA5" s="2">
+        <v>44457.52199074074</v>
+      </c>
+      <c r="AB5">
+        <v>109</v>
+      </c>
+      <c r="AC5">
         <v>108</v>
       </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="s">
-        <v>45</v>
-      </c>
-      <c r="J5" s="2">
-        <v>44457.52199074074</v>
-      </c>
-      <c r="K5" s="2">
-        <v>44459.5591087963</v>
-      </c>
-      <c r="L5" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" t="s">
-        <v>47</v>
-      </c>
-      <c r="N5" s="2">
-        <v>44456.52199074074</v>
-      </c>
-      <c r="P5" t="s">
-        <v>51</v>
-      </c>
-      <c r="S5" t="s">
-        <v>55</v>
-      </c>
-      <c r="T5" t="s">
-        <v>59</v>
-      </c>
-      <c r="U5" t="s">
-        <v>59</v>
-      </c>
-      <c r="V5" t="s">
+      <c r="AD5" t="s">
         <v>61</v>
       </c>
-      <c r="W5">
-        <v>1024</v>
-      </c>
-      <c r="Y5">
-        <v>106</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC5">
-        <v>109</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>63</v>
-      </c>
       <c r="AE5" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="AF5" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="AG5">
         <v>106</v>
@@ -1118,12 +1124,6 @@
         <v>44459.54693287037</v>
       </c>
       <c r="AI5" t="s">
-        <v>68</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1142,22 +1142,22 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>74</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -1165,19 +1165,19 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
         <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -1185,19 +1185,19 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
         <v>76</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1205,19 +1205,19 @@
         <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D4" t="s">
         <v>75</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G4" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -1225,19 +1225,19 @@
         <v>108</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -1245,19 +1245,19 @@
         <v>109</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
         <v>77</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1265,19 +1265,19 @@
         <v>110</v>
       </c>
       <c r="B7" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D7" t="s">
         <v>78</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -1285,22 +1285,22 @@
         <v>111</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D8" t="s">
         <v>79</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -1308,22 +1308,22 @@
         <v>112</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D9" t="s">
         <v>80</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -1331,22 +1331,22 @@
         <v>113</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D10" t="s">
         <v>81</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -1354,19 +1354,19 @@
         <v>114</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -1374,22 +1374,22 @@
         <v>115</v>
       </c>
       <c r="B12" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -1397,19 +1397,19 @@
         <v>116</v>
       </c>
       <c r="B13" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
         <v>75</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G13" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1417,19 +1417,19 @@
         <v>117</v>
       </c>
       <c r="B14" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
         <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G14" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -1437,19 +1437,19 @@
         <v>118</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
         <v>77</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G15" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -1457,19 +1457,19 @@
         <v>119</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
         <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:7">
@@ -1477,22 +1477,22 @@
         <v>120</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
         <v>79</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G17" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:7">
@@ -1500,22 +1500,22 @@
         <v>121</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
         <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F18" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G18" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7">
@@ -1523,22 +1523,22 @@
         <v>122</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
         <v>81</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G19" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:7">
@@ -1546,19 +1546,19 @@
         <v>123</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
         <v>82</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G20" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="21" spans="1:7">
@@ -1566,22 +1566,22 @@
         <v>124</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
         <v>83</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F21" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:7">
@@ -1589,19 +1589,19 @@
         <v>125</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C22" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D22" t="s">
         <v>75</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G22" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:7">
@@ -1609,19 +1609,19 @@
         <v>126</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D23" t="s">
         <v>76</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G23" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1629,19 +1629,19 @@
         <v>127</v>
       </c>
       <c r="B24" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D24" t="s">
         <v>77</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G24" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:7">
@@ -1649,19 +1649,19 @@
         <v>128</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D25" t="s">
         <v>78</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G25" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1669,22 +1669,22 @@
         <v>129</v>
       </c>
       <c r="B26" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D26" t="s">
         <v>79</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F26" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G26" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:7">
@@ -1692,22 +1692,22 @@
         <v>130</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C27" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D27" t="s">
         <v>80</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F27" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G27" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:7">
@@ -1715,22 +1715,22 @@
         <v>131</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C28" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
         <v>81</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F28" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G28" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:7">
@@ -1738,19 +1738,19 @@
         <v>132</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D29" t="s">
         <v>82</v>
       </c>
       <c r="E29" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="G29" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1758,22 +1758,22 @@
         <v>133</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="C30" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
         <v>83</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
       <c r="F30" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="G30" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>